<commit_message>
Atividade 4 menos printar caminho vertice a raiz
</commit_message>
<xml_diff>
--- a/docs/Grafos/Grafos.xlsx
+++ b/docs/Grafos/Grafos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Documents\Cience Computing\Unifor\Trabalhos\Resolução de problemas com grafos\grafosPy\docs\Grafos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jafer\Documents\Grafos\grafosPy\docs\Grafos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9613B14B-D6B6-42A6-AFC9-F8DA23E72A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB5E0E4-457F-4340-8428-1A143216B5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grafo 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Grafo 3" sheetId="3" r:id="rId3"/>
     <sheet name="Grafo 4" sheetId="4" r:id="rId4"/>
     <sheet name="Grafo 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Grafo 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="A">'Grafo 4'!$1:$1</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="11">
   <si>
     <t>V</t>
   </si>
@@ -507,17 +508,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="2.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="2.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -569,7 +570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -595,7 +596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -621,7 +622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -647,7 +648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -673,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -699,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -739,16 +740,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="2.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="2.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -774,7 +775,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -800,7 +801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -826,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -852,7 +853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -878,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -904,7 +905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -930,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -970,17 +971,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="2.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="2.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1015,7 +1016,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1050,7 +1051,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1085,7 +1086,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1120,7 +1121,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1155,7 +1156,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1190,7 +1191,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1225,7 +1226,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="7"/>
     </row>
-    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1276,16 +1277,16 @@
       <selection sqref="A1:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="2.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="2.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1311,7 +1312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1337,7 +1338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1363,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1389,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1415,7 +1416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1441,7 +1442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1467,7 +1468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1502,21 +1503,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA27B47-58E8-44CC-8638-FA8B7F973EF0}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="A1:K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="2.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="2.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="2.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1551,7 +1552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1586,7 +1587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1621,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1656,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1691,7 +1692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1726,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1761,7 +1762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1796,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
@@ -1831,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
@@ -1866,7 +1867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
@@ -1901,8 +1902,151 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="S16" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852D2AB0-639F-4F31-A20E-8D9DDE98AF7F}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
criação grafo atividade 5
</commit_message>
<xml_diff>
--- a/docs/Grafos/Grafos.xlsx
+++ b/docs/Grafos/Grafos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jafer\Documents\Grafos\grafosPy\docs\Grafos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Documents\Cience Computing\Unifor\Trabalhos\Resolução de problemas com grafos\grafosPy\docs\Grafos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB5E0E4-457F-4340-8428-1A143216B5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE0BD6F-A081-4E8A-BDCE-07EE6D046FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grafo 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Grafo 4" sheetId="4" r:id="rId4"/>
     <sheet name="Grafo 5" sheetId="5" r:id="rId5"/>
     <sheet name="Grafo 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Grafo 7" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="A">'Grafo 4'!$1:$1</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="11">
   <si>
     <t>V</t>
   </si>
@@ -508,17 +509,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="2.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="2.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +545,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -570,7 +571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -596,7 +597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -622,7 +623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -648,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -674,7 +675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -700,7 +701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -740,16 +741,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="2.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="2.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -801,7 +802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -827,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -853,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -879,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -905,7 +906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -931,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -971,17 +972,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="2.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="2.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1017,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1051,7 +1052,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1086,7 +1087,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1121,7 +1122,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1156,7 +1157,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1191,7 +1192,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1226,7 +1227,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="7"/>
     </row>
-    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1274,19 +1275,19 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H8"/>
+      <selection sqref="A1:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="2.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="2.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1312,7 +1313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1338,7 +1339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1364,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1390,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1416,7 +1417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1442,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1468,7 +1469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1504,20 +1505,20 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="A1:K11"/>
+      <selection sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="2.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1587,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1622,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1657,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1692,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1797,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
@@ -1832,7 +1833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
@@ -1867,7 +1868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
@@ -1902,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S16" s="11"/>
     </row>
   </sheetData>
@@ -1915,19 +1916,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852D2AB0-639F-4F31-A20E-8D9DDE98AF7F}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1947,7 +1948,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1967,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1987,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2007,7 +2008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2027,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -2047,6 +2048,293 @@
         <v>0</v>
       </c>
       <c r="G6" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B425FED9-951C-48A8-9087-46D6B84B43E9}">
+  <dimension ref="A1:N12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="2.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N12" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Adição de grafos direcionados
</commit_message>
<xml_diff>
--- a/docs/Grafos/Grafos.xlsx
+++ b/docs/Grafos/Grafos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Documents\Cience Computing\Unifor\Trabalhos\Resolução de problemas com grafos\grafosPy\docs\Grafos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE0BD6F-A081-4E8A-BDCE-07EE6D046FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0E0E27-7DBE-4682-B47E-0A4BD37355C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7785" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grafo 1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="Grafo 5" sheetId="5" r:id="rId5"/>
     <sheet name="Grafo 6" sheetId="6" r:id="rId6"/>
     <sheet name="Grafo 7" sheetId="7" r:id="rId7"/>
+    <sheet name="Grafo 8" sheetId="8" r:id="rId8"/>
+    <sheet name="Grafo 9" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="A">'Grafo 4'!$1:$1</definedName>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="15">
   <si>
     <t>V</t>
   </si>
@@ -63,6 +65,18 @@
   </si>
   <si>
     <t>J</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1504,7 +1518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA27B47-58E8-44CC-8638-FA8B7F973EF0}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
@@ -1916,7 +1930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852D2AB0-639F-4F31-A20E-8D9DDE98AF7F}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -2059,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B425FED9-951C-48A8-9087-46D6B84B43E9}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2340,4 +2354,951 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45CE7454-4D6F-4EDD-AF13-4F5A07146950}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>5</v>
+      </c>
+      <c r="H5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>4</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE53B129-FB93-4F5C-A142-1B714C795DF3}">
+  <dimension ref="A1:O18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>2</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>9</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>3</v>
+      </c>
+      <c r="H4" s="4">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>6</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+      <c r="O5" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>8</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4">
+        <v>6</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <v>4</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>7</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>10</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>13</v>
+      </c>
+      <c r="M11" s="4">
+        <v>8</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0</v>
+      </c>
+      <c r="L14" s="4">
+        <v>9</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>6</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>